<commit_message>
Apart soort expanded output, print voor department + verbeteringen
</commit_message>
<xml_diff>
--- a/model/Data assignment operating room 2 Large.xlsx
+++ b/model/Data assignment operating room 2 Large.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tip\Documents\GitHub\modellingb\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3039D9-EDC2-4F83-B72C-ED8F3AF3F59B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D373D7E-E481-46AC-A31A-91D0080ED59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>Number operating rooms</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Overtime per department</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -443,7 +452,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +585,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -587,7 +596,7 @@
         <v>171</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -598,7 +607,7 @@
         <v>125</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -609,7 +618,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -620,7 +629,7 @@
         <v>127</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -631,7 +640,7 @@
         <v>65</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -642,7 +651,7 @@
         <v>60</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -653,7 +662,7 @@
         <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -664,7 +673,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -675,7 +684,7 @@
         <v>121</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -686,7 +695,7 @@
         <v>51</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -697,7 +706,7 @@
         <v>61</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -708,7 +717,7 @@
         <v>262</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -719,7 +728,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,7 +739,7 @@
         <v>102</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -741,7 +750,7 @@
         <v>82</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -752,7 +761,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -763,7 +772,7 @@
         <v>50</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -774,7 +783,7 @@
         <v>74</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -785,7 +794,7 @@
         <v>40</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -796,7 +805,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -807,7 +816,7 @@
         <v>324</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,7 +827,7 @@
         <v>324</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -829,7 +838,7 @@
         <v>46</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -840,7 +849,7 @@
         <v>125</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>